<commit_message>
Planning.xlsx bijgewerkt + nu documenten toegevoegd
</commit_message>
<xml_diff>
--- a/documenten/Planning.xlsx
+++ b/documenten/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>week 38</t>
   </si>
@@ -60,34 +60,61 @@
     <t>week 51</t>
   </si>
   <si>
-    <t>overzicht bestellingen</t>
-  </si>
-  <si>
-    <t>layout website</t>
-  </si>
-  <si>
-    <t>categorie Beheer</t>
-  </si>
-  <si>
-    <t>Merk Beheer</t>
-  </si>
-  <si>
-    <t>Contact Pagina</t>
-  </si>
-  <si>
     <t>Login / logout</t>
   </si>
   <si>
-    <t>KlAc overzicht Bestellingen *</t>
-  </si>
-  <si>
-    <t>KlAc wachtwoord wijzigen *</t>
-  </si>
-  <si>
-    <t>KlAc adres gegevens wijzigen *</t>
-  </si>
-  <si>
-    <t>Database Opstellen</t>
+    <t>Bestellen</t>
+  </si>
+  <si>
+    <t>Door producten kijken</t>
+  </si>
+  <si>
+    <t>* KA = Klant Account</t>
+  </si>
+  <si>
+    <t>KA wachtwoord wijzigen *</t>
+  </si>
+  <si>
+    <t>KA adres gegevens wijzigen *</t>
+  </si>
+  <si>
+    <t>Overzicht bestellingen</t>
+  </si>
+  <si>
+    <t>Product beheer</t>
+  </si>
+  <si>
+    <t>Merk beheer</t>
+  </si>
+  <si>
+    <t>Categorie beheer</t>
+  </si>
+  <si>
+    <t>KA overzicht bestellingen *</t>
+  </si>
+  <si>
+    <t>Contact pagina</t>
+  </si>
+  <si>
+    <t>Layout website</t>
+  </si>
+  <si>
+    <t>Database opstellen</t>
+  </si>
+  <si>
+    <t>Algemeen =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerrit de Groot = </t>
+  </si>
+  <si>
+    <t>Timon de Groot =</t>
+  </si>
+  <si>
+    <t>Acceptatie test</t>
+  </si>
+  <si>
+    <t>Afwerken / Optionele functies</t>
   </si>
 </sst>
 </file>
@@ -103,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,18 +151,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -148,25 +163,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -195,6 +234,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -496,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,13 +595,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -579,68 +620,119 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
functioneel ontwerp met schermontwerp
</commit_message>
<xml_diff>
--- a/documenten/Planning.xlsx
+++ b/documenten/Planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>week 38</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Afwerken / Optionele functies</t>
-  </si>
-  <si>
-    <t>Registratie</t>
   </si>
 </sst>
 </file>
@@ -543,7 +540,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,115 +626,109 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="11"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>

</xml_diff>